<commit_message>
config.ymal had its case sensitivity tweaked
</commit_message>
<xml_diff>
--- a/data/costs.xlsx
+++ b/data/costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myles\OneDrive\Desktop\DEMO - Dashboard\my-project-demo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0932A30-648A-45F3-84DF-17E0BCE0DF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A187EE51-36C8-4818-BDA4-8C3C7F6B532C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3768" yWindow="3756" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2112" yWindow="3720" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -129,12 +129,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,45 +424,45 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3">
@@ -488,7 +488,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -514,7 +514,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5">
@@ -540,7 +540,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6">

</xml_diff>